<commit_message>
Added new data sets, raised accuracy
</commit_message>
<xml_diff>
--- a/data/masterSet.xlsx
+++ b/data/masterSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Desktop\Spring-Research-2022\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD04F314-D94A-4B1A-A918-95AE22B6C58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5E6C04-F881-4627-B489-90BD029A94CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="13">
   <si>
     <t>Channel</t>
   </si>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,6 +1614,790 @@
         <v>0</v>
       </c>
     </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <v>139.30464912377872</v>
+      </c>
+      <c r="C82">
+        <v>921.6391379649823</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83">
+        <v>133.51868036160101</v>
+      </c>
+      <c r="C83">
+        <v>682.65556698579053</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84">
+        <v>92.875948209028977</v>
+      </c>
+      <c r="C84">
+        <v>714.06440672507654</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85">
+        <v>114.37112615658687</v>
+      </c>
+      <c r="C85">
+        <v>422.89784820263202</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86">
+        <v>85.312759784551773</v>
+      </c>
+      <c r="C86">
+        <v>457.77465798304632</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>59.447127470603355</v>
+      </c>
+      <c r="C87">
+        <v>264.57460381434515</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88">
+        <v>134.35369909726657</v>
+      </c>
+      <c r="C88">
+        <v>331.53298466022198</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89">
+        <v>60.747052394426788</v>
+      </c>
+      <c r="C89">
+        <v>278.24108285170337</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90">
+        <v>17.734175828786995</v>
+      </c>
+      <c r="C90">
+        <v>15.76536618746244</v>
+      </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91">
+        <v>16.679549437302811</v>
+      </c>
+      <c r="C91">
+        <v>17.642024553739109</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92">
+        <v>19.761544594397911</v>
+      </c>
+      <c r="C92">
+        <v>21.199544173020584</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93">
+        <v>20.361760799701397</v>
+      </c>
+      <c r="C93">
+        <v>17.875503466679501</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94">
+        <v>21.0097226362962</v>
+      </c>
+      <c r="C94">
+        <v>15.958862231327938</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95">
+        <v>42.094740794255181</v>
+      </c>
+      <c r="C95">
+        <v>15.279813913198618</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96">
+        <v>19.872208081758938</v>
+      </c>
+      <c r="C96">
+        <v>13.41997109926664</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97">
+        <v>32.27365537790152</v>
+      </c>
+      <c r="C97">
+        <v>22.17827320098877</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98">
+        <v>10.984649364764874</v>
+      </c>
+      <c r="C98">
+        <v>7.3801723844729938</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99">
+        <v>43.437601749713608</v>
+      </c>
+      <c r="C99">
+        <v>17.10391715856699</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100">
+        <v>15.946001254595243</v>
+      </c>
+      <c r="C100">
+        <v>10.220108740604841</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101">
+        <v>12.259904678051289</v>
+      </c>
+      <c r="C101">
+        <v>10.030653958137218</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102">
+        <v>43.637437306917633</v>
+      </c>
+      <c r="C102">
+        <v>23.242417107407864</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <v>50.297773810533378</v>
+      </c>
+      <c r="C103">
+        <v>10.180087707936764</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104">
+        <v>11.398828423940218</v>
+      </c>
+      <c r="C104">
+        <v>9.0864980197869816</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>10</v>
+      </c>
+      <c r="B105">
+        <v>34.465603702343429</v>
+      </c>
+      <c r="C105">
+        <v>9.6959857677037906</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>37.577071432883926</v>
+      </c>
+      <c r="C106">
+        <v>10.336478711320805</v>
+      </c>
+      <c r="D106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>9</v>
+      </c>
+      <c r="B107">
+        <v>20.580863154851475</v>
+      </c>
+      <c r="C107">
+        <v>7.2496556421885128</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>10</v>
+      </c>
+      <c r="B108">
+        <v>45.140778720378876</v>
+      </c>
+      <c r="C108">
+        <v>6.7889590011193199</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109">
+        <v>35.592536733700676</v>
+      </c>
+      <c r="C109">
+        <v>6.8021187243553305</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110">
+        <v>46.739307637398056</v>
+      </c>
+      <c r="C110">
+        <v>10.987723417007006</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111">
+        <v>35.884697350171898</v>
+      </c>
+      <c r="C111">
+        <v>11.033881172537804</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112">
+        <v>26.148272943038208</v>
+      </c>
+      <c r="C112">
+        <v>7.5593141718552666</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>10</v>
+      </c>
+      <c r="B113">
+        <v>26.662141859531403</v>
+      </c>
+      <c r="C113">
+        <v>8.6836000428749962</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114">
+        <v>66.342754134765045</v>
+      </c>
+      <c r="C114">
+        <v>13.0430716918065</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115">
+        <v>67.357748590982879</v>
+      </c>
+      <c r="C115">
+        <v>10.095222266820761</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>10</v>
+      </c>
+      <c r="B116">
+        <v>61.879314853594856</v>
+      </c>
+      <c r="C116">
+        <v>8.1855825999608403</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117">
+        <v>46.610791355371475</v>
+      </c>
+      <c r="C117">
+        <v>11.350654348731041</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118">
+        <v>51.166381372855263</v>
+      </c>
+      <c r="C118">
+        <v>8.4160332301488285</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119">
+        <v>62.964724467350884</v>
+      </c>
+      <c r="C119">
+        <v>11.448315840501051</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120">
+        <v>52.84523785802034</v>
+      </c>
+      <c r="C120">
+        <v>9.9696730535763969</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>10</v>
+      </c>
+      <c r="B121">
+        <v>77.908704138719116</v>
+      </c>
+      <c r="C121">
+        <v>9.3947173609183388</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122">
+        <v>32.858189431520607</v>
+      </c>
+      <c r="C122">
+        <v>5.0025127931283073</v>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123">
+        <v>51.641768840643074</v>
+      </c>
+      <c r="C123">
+        <v>4.5084924984436769</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>10</v>
+      </c>
+      <c r="B124">
+        <v>50.78301159005899</v>
+      </c>
+      <c r="C124">
+        <v>9.5494402394844933</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>12</v>
+      </c>
+      <c r="B125">
+        <v>28.867430583788799</v>
+      </c>
+      <c r="C125">
+        <v>4.8104356378316879</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>12</v>
+      </c>
+      <c r="B126">
+        <v>21.107921126943367</v>
+      </c>
+      <c r="C126">
+        <v>3.8491739447300253</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127">
+        <v>13.486887950163622</v>
+      </c>
+      <c r="C127">
+        <v>2.8865842211704988</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>9</v>
+      </c>
+      <c r="B128">
+        <v>18.927964623157795</v>
+      </c>
+      <c r="C128">
+        <v>4.0615977335434694</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129">
+        <v>16.830797405197071</v>
+      </c>
+      <c r="C129">
+        <v>3.2112299971855602</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130">
+        <v>19.396602043738731</v>
+      </c>
+      <c r="C130">
+        <v>11.061275019095493</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>9</v>
+      </c>
+      <c r="B131">
+        <v>36.426098080781792</v>
+      </c>
+      <c r="C131">
+        <v>9.3817504094197197</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>10</v>
+      </c>
+      <c r="B132">
+        <v>40.917258088405319</v>
+      </c>
+      <c r="C132">
+        <v>12.612592224891369</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133">
+        <v>28.658360536281879</v>
+      </c>
+      <c r="C133">
+        <v>9.9017491432336655</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134">
+        <v>34.38826078634996</v>
+      </c>
+      <c r="C134">
+        <v>13.508753666510948</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>4</v>
+      </c>
+      <c r="B135">
+        <v>29.271822892702541</v>
+      </c>
+      <c r="C135">
+        <v>11.188973656067482</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>9</v>
+      </c>
+      <c r="B136">
+        <v>29.971125052525448</v>
+      </c>
+      <c r="C136">
+        <v>11.510829017712521</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>10</v>
+      </c>
+      <c r="B137">
+        <v>41.808013365818901</v>
+      </c>
+      <c r="C137">
+        <v>11.297479125169607</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>